<commit_message>
Removed the start and end tags from the resource's "text.`div`" field when displayed in a table
LF-3428
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions-R4.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions-R4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\lhc-lx-ftdev04\sedinkinya\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D6AEB-AD12-4DCA-A394-CEF3E08DD8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325D1FEB-D406-4F49-A6D1-850AE0D87AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2955" yWindow="2190" windowWidth="36585" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4938,9 +4938,6 @@
     <t>Section 1 Text</t>
   </si>
   <si>
-    <t>section[0].text.`div`</t>
-  </si>
-  <si>
     <t>section[0].title</t>
   </si>
   <si>
@@ -4954,6 +4951,9 @@
   </si>
   <si>
     <t>section-1-text</t>
+  </si>
+  <si>
+    <t>section[0].text.`div`.select(iif(matches('^(&lt;\\?xml [^&gt;]*&gt;|)&lt;div( [^&gt;]*|)&gt;(.*)&lt;/div&gt;$'), replaceMatches('^(&lt;\\?xml [^&gt;]*&gt;|)&lt;div( [^&gt;]*|)&gt;(.*)&lt;/div&gt;$', '$3'), $this))</t>
   </si>
 </sst>
 </file>
@@ -5365,7 +5365,7 @@
   <dimension ref="A1:H431"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6004,7 +6004,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>36</v>
@@ -6019,16 +6019,16 @@
         <v>33</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>1639</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>1640</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>36</v>
@@ -6043,10 +6043,10 @@
         <v>33</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>1638</v>
+        <v>1643</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add the columns "Age" and "State" to the patients table
LF-3447

Also, added unit tests, and fixed a potential bug identified by these tests
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions-R4.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions-R4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\lhc-lx-ftdev04\sedinkinya\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325D1FEB-D406-4F49-A6D1-850AE0D87AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA4273E-61BD-4C7C-8352-DF619034E917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="2190" windowWidth="36585" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6405" yWindow="2175" windowWidth="36585" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources on LForms R4 server" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10378" uniqueCount="1644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10392" uniqueCount="1652">
   <si>
     <t>Legend</t>
   </si>
@@ -4954,6 +4954,30 @@
   </si>
   <si>
     <t>section[0].text.`div`.select(iif(matches('^(&lt;\\?xml [^&gt;]*&gt;|)&lt;div( [^&gt;]*|)&gt;(.*)&lt;/div&gt;$'), replaceMatches('^(&lt;\\?xml [^&gt;]*&gt;|)&lt;div( [^&gt;]*|)&gt;(.*)&lt;/div&gt;$', '$3'), $this))</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>The patient's age</t>
+  </si>
+  <si>
+    <t>iif(birthDate.exists(), defineVariable('referenceDate', iif(%context.deceasedDateTime.exists(), %context.deceasedDateTime, today())).select((%referenceDate.toString().substring(0,4).toInteger() - %context.birthDate.toString().substring(0,4).toInteger()) - iif(%referenceDate.toString().substring(5,10) &lt; %context.birthDate.toString().substring(5,10),1,0)), {})</t>
+  </si>
+  <si>
+    <t>unsignedInt</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>defineVariable('homeAddress', address.where(use = 'home')).select(iif(%homeAddress.exists(), %homeAddress, address)).state.first()</t>
+  </si>
+  <si>
+    <t>State (from the first possible home address where the state is specified)</t>
   </si>
 </sst>
 </file>
@@ -5362,10 +5386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H431"/>
+  <dimension ref="A1:H433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
+      <selection activeCell="G396" sqref="G396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13389,34 +13413,38 @@
       </c>
     </row>
     <row r="396" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B396" t="s">
-        <v>657</v>
-      </c>
-      <c r="C396" t="s">
-        <v>18</v>
-      </c>
-      <c r="D396" t="s">
-        <v>658</v>
-      </c>
-      <c r="E396" t="s">
-        <v>20</v>
-      </c>
-      <c r="F396" t="s">
+      <c r="A396" s="2"/>
+      <c r="B396" s="2" t="s">
+        <v>1648</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E396" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F396" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H396" t="s">
-        <v>659</v>
+      <c r="G396" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="H396" s="2" t="s">
+        <v>1651</v>
       </c>
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C397" t="s">
         <v>18</v>
       </c>
       <c r="D397" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="E397" t="s">
         <v>20</v>
@@ -13425,18 +13453,18 @@
         <v>33</v>
       </c>
       <c r="H397" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C398" t="s">
         <v>18</v>
       </c>
       <c r="D398" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E398" t="s">
         <v>20</v>
@@ -13445,18 +13473,18 @@
         <v>33</v>
       </c>
       <c r="H398" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C399" t="s">
         <v>18</v>
       </c>
       <c r="D399" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="E399" t="s">
         <v>20</v>
@@ -13465,103 +13493,101 @@
         <v>33</v>
       </c>
       <c r="H399" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C400" t="s">
         <v>18</v>
       </c>
       <c r="D400" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="E400" t="s">
         <v>20</v>
       </c>
       <c r="F400" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="H400" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
+        <v>669</v>
+      </c>
+      <c r="C401" t="s">
+        <v>18</v>
+      </c>
+      <c r="D401" t="s">
+        <v>670</v>
+      </c>
+      <c r="E401" t="s">
+        <v>20</v>
+      </c>
+      <c r="F401" t="s">
+        <v>62</v>
+      </c>
+      <c r="H401" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B402" t="s">
         <v>672</v>
       </c>
-      <c r="C401" t="s">
-        <v>18</v>
-      </c>
-      <c r="D401" t="s">
+      <c r="C402" t="s">
+        <v>18</v>
+      </c>
+      <c r="D402" t="s">
         <v>672</v>
       </c>
-      <c r="E401" t="s">
-        <v>20</v>
-      </c>
-      <c r="F401" t="s">
+      <c r="E402" t="s">
+        <v>20</v>
+      </c>
+      <c r="F402" t="s">
         <v>29</v>
       </c>
-      <c r="H401" t="s">
+      <c r="H402" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A402" s="3"/>
-      <c r="B402" s="3" t="s">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A403" s="3"/>
+      <c r="B403" s="3" t="s">
         <v>674</v>
       </c>
-      <c r="C402" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D402" s="3" t="s">
+      <c r="C403" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D403" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="E402" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F402" s="3" t="s">
+      <c r="E403" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F403" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G402" s="3"/>
-      <c r="H402" s="3" t="s">
+      <c r="G403" s="3"/>
+      <c r="H403" s="3" t="s">
         <v>676</v>
-      </c>
-    </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A403" s="4"/>
-      <c r="B403" s="4" t="s">
-        <v>677</v>
-      </c>
-      <c r="C403" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D403" s="4" t="s">
-        <v>678</v>
-      </c>
-      <c r="E403" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F403" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G403" s="4"/>
-      <c r="H403" s="4" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A404" s="4"/>
       <c r="B404" s="4" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="C404" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D404" s="4" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E404" s="4" t="s">
         <v>24</v>
@@ -13571,568 +13597,614 @@
       </c>
       <c r="G404" s="4"/>
       <c r="H404" s="4" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A405" s="4"/>
+      <c r="B405" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="C405" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D405" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="E405" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F405" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G405" s="4"/>
+      <c r="H405" s="4" t="s">
         <v>682</v>
-      </c>
-    </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B405" t="s">
-        <v>683</v>
-      </c>
-      <c r="C405" t="s">
-        <v>18</v>
-      </c>
-      <c r="D405" t="s">
-        <v>684</v>
-      </c>
-      <c r="E405" t="s">
-        <v>24</v>
-      </c>
-      <c r="F405" t="s">
-        <v>107</v>
-      </c>
-      <c r="H405" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
+        <v>683</v>
+      </c>
+      <c r="C406" t="s">
+        <v>18</v>
+      </c>
+      <c r="D406" t="s">
+        <v>684</v>
+      </c>
+      <c r="E406" t="s">
+        <v>24</v>
+      </c>
+      <c r="F406" t="s">
+        <v>107</v>
+      </c>
+      <c r="H406" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B407" t="s">
         <v>686</v>
       </c>
-      <c r="C406" t="s">
-        <v>18</v>
-      </c>
-      <c r="D406" t="s">
+      <c r="C407" t="s">
+        <v>18</v>
+      </c>
+      <c r="D407" t="s">
         <v>686</v>
       </c>
-      <c r="E406" t="s">
-        <v>20</v>
-      </c>
-      <c r="F406" t="s">
+      <c r="E407" t="s">
+        <v>20</v>
+      </c>
+      <c r="F407" t="s">
         <v>391</v>
       </c>
-      <c r="H406" t="s">
+      <c r="H407" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A407" s="3"/>
-      <c r="B407" s="3" t="s">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A408" s="3"/>
+      <c r="B408" s="3" t="s">
         <v>688</v>
       </c>
-      <c r="C407" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D407" s="3" t="s">
+      <c r="C408" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D408" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="E407" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F407" s="3" t="s">
+      <c r="E408" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F408" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="G407" s="3"/>
-      <c r="H407" s="3" t="s">
+      <c r="G408" s="3"/>
+      <c r="H408" s="3" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B408" t="s">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A409" s="2"/>
+      <c r="B409" s="2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E409" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F409" s="2" t="s">
+        <v>1647</v>
+      </c>
+      <c r="G409" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="H409" s="2" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B410" t="s">
         <v>692</v>
       </c>
-      <c r="C408" t="s">
-        <v>18</v>
-      </c>
-      <c r="D408" t="s">
+      <c r="C410" t="s">
+        <v>18</v>
+      </c>
+      <c r="D410" t="s">
         <v>692</v>
       </c>
-      <c r="E408" t="s">
-        <v>20</v>
-      </c>
-      <c r="F408" t="s">
+      <c r="E410" t="s">
+        <v>20</v>
+      </c>
+      <c r="F410" t="s">
         <v>693</v>
       </c>
-      <c r="H408" t="s">
+      <c r="H410" t="s">
         <v>694</v>
-      </c>
-    </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B409" t="s">
-        <v>695</v>
-      </c>
-      <c r="C409" t="s">
-        <v>18</v>
-      </c>
-      <c r="D409" t="s">
-        <v>695</v>
-      </c>
-      <c r="E409" t="s">
-        <v>20</v>
-      </c>
-      <c r="F409" t="s">
-        <v>33</v>
-      </c>
-      <c r="H409" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A410" s="3"/>
-      <c r="B410" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="C410" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D410" s="3" t="s">
-        <v>698</v>
-      </c>
-      <c r="E410" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F410" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G410" s="3"/>
-      <c r="H410" s="3" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="411" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
+        <v>695</v>
+      </c>
+      <c r="C411" t="s">
+        <v>18</v>
+      </c>
+      <c r="D411" t="s">
+        <v>695</v>
+      </c>
+      <c r="E411" t="s">
+        <v>20</v>
+      </c>
+      <c r="F411" t="s">
+        <v>33</v>
+      </c>
+      <c r="H411" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A412" s="3"/>
+      <c r="B412" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="C411" t="s">
-        <v>18</v>
-      </c>
-      <c r="D411" t="s">
+      <c r="C412" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D412" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="E412" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F412" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G412" s="3"/>
+      <c r="H412" s="3" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B413" t="s">
         <v>697</v>
       </c>
-      <c r="E411" t="s">
-        <v>20</v>
-      </c>
-      <c r="F411" t="s">
+      <c r="C413" t="s">
+        <v>18</v>
+      </c>
+      <c r="D413" t="s">
+        <v>697</v>
+      </c>
+      <c r="E413" t="s">
+        <v>20</v>
+      </c>
+      <c r="F413" t="s">
         <v>62</v>
       </c>
-      <c r="H411" t="s">
+      <c r="H413" t="s">
         <v>700</v>
-      </c>
-    </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B412" t="s">
-        <v>701</v>
-      </c>
-      <c r="C412" t="s">
-        <v>18</v>
-      </c>
-      <c r="D412" t="s">
-        <v>702</v>
-      </c>
-      <c r="E412" t="s">
-        <v>24</v>
-      </c>
-      <c r="F412" t="s">
-        <v>41</v>
-      </c>
-      <c r="H412" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A413" s="4"/>
-      <c r="B413" s="4" t="s">
-        <v>704</v>
-      </c>
-      <c r="C413" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D413" s="4" t="s">
-        <v>705</v>
-      </c>
-      <c r="E413" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F413" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G413" s="4"/>
-      <c r="H413" s="4" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="C414" t="s">
         <v>18</v>
       </c>
       <c r="D414" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E414" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F414" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H414" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="415" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A415" s="3"/>
-      <c r="B415" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C415" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D415" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E415" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F415" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G415" s="3"/>
-      <c r="H415" s="3"/>
+      <c r="A415" s="4"/>
+      <c r="B415" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="C415" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D415" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="E415" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F415" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G415" s="4"/>
+      <c r="H415" s="4" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="416" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>79</v>
+        <v>707</v>
       </c>
       <c r="C416" t="s">
         <v>18</v>
       </c>
       <c r="D416" t="s">
-        <v>79</v>
+        <v>707</v>
       </c>
       <c r="E416" t="s">
         <v>20</v>
       </c>
       <c r="F416" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="H416" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="417" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A417" s="3"/>
       <c r="B417" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C417" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D417" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E417" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F417" s="3" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="G417" s="3"/>
-      <c r="H417" s="3" t="s">
-        <v>710</v>
-      </c>
+      <c r="H417" s="3"/>
     </row>
     <row r="418" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
+        <v>79</v>
+      </c>
+      <c r="C418" t="s">
+        <v>18</v>
+      </c>
+      <c r="D418" t="s">
+        <v>79</v>
+      </c>
+      <c r="E418" t="s">
+        <v>20</v>
+      </c>
+      <c r="F418" t="s">
+        <v>80</v>
+      </c>
+      <c r="H418" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A419" s="3"/>
+      <c r="B419" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C419" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D419" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E419" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F419" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G419" s="3"/>
+      <c r="H419" s="3" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B420" t="s">
         <v>163</v>
       </c>
-      <c r="C418" t="s">
-        <v>18</v>
-      </c>
-      <c r="D418" t="s">
+      <c r="C420" t="s">
+        <v>18</v>
+      </c>
+      <c r="D420" t="s">
         <v>163</v>
       </c>
-      <c r="E418" t="s">
-        <v>24</v>
-      </c>
-      <c r="F418" t="s">
+      <c r="E420" t="s">
+        <v>24</v>
+      </c>
+      <c r="F420" t="s">
         <v>47</v>
       </c>
-      <c r="H418" t="s">
+      <c r="H420" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B419" t="s">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B421" t="s">
         <v>712</v>
       </c>
-      <c r="C419" t="s">
-        <v>18</v>
-      </c>
-      <c r="D419" t="s">
+      <c r="C421" t="s">
+        <v>18</v>
+      </c>
+      <c r="D421" t="s">
         <v>712</v>
       </c>
-      <c r="E419" t="s">
-        <v>24</v>
-      </c>
-      <c r="F419" t="s">
+      <c r="E421" t="s">
+        <v>24</v>
+      </c>
+      <c r="F421" t="s">
         <v>41</v>
       </c>
-      <c r="H419" t="s">
+      <c r="H421" t="s">
         <v>713</v>
-      </c>
-    </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A420" s="4"/>
-      <c r="B420" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="C420" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D420" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="E420" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F420" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G420" s="4"/>
-      <c r="H420" s="4" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A421" s="4"/>
-      <c r="B421" s="4" t="s">
-        <v>716</v>
-      </c>
-      <c r="C421" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D421" s="4" t="s">
-        <v>717</v>
-      </c>
-      <c r="E421" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F421" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G421" s="4"/>
-      <c r="H421" s="4" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="422" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A422" s="4"/>
       <c r="B422" s="4" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="C422" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D422" s="4" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="E422" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F422" s="4" t="s">
-        <v>47</v>
+      <c r="F422" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="G422" s="4"/>
       <c r="H422" s="4" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
     </row>
     <row r="423" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A423" s="4"/>
       <c r="B423" s="4" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="C423" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D423" s="4" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="E423" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F423" s="4" t="s">
-        <v>724</v>
+        <v>44</v>
       </c>
       <c r="G423" s="4"/>
       <c r="H423" s="4" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A424" s="4"/>
+      <c r="B424" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="C424" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D424" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="E424" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F424" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G424" s="4"/>
+      <c r="H424" s="4" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A425" s="4"/>
+      <c r="B425" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="C425" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D425" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="E425" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F425" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="G425" s="4"/>
+      <c r="H425" s="4" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A424" s="3"/>
-      <c r="B424" s="3" t="s">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A426" s="3"/>
+      <c r="B426" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C424" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D424" s="3" t="s">
+      <c r="C426" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D426" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E424" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F424" s="3" t="s">
+      <c r="E426" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F426" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="G424" s="3"/>
-      <c r="H424" s="3" t="s">
+      <c r="G426" s="3"/>
+      <c r="H426" s="3" t="s">
         <v>727</v>
-      </c>
-    </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B425" t="s">
-        <v>288</v>
-      </c>
-      <c r="C425" t="s">
-        <v>18</v>
-      </c>
-      <c r="D425" t="s">
-        <v>288</v>
-      </c>
-      <c r="E425" t="s">
-        <v>20</v>
-      </c>
-      <c r="F425" t="s">
-        <v>33</v>
-      </c>
-      <c r="H425" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B426" t="s">
-        <v>729</v>
-      </c>
-      <c r="C426" t="s">
-        <v>18</v>
-      </c>
-      <c r="D426" t="s">
-        <v>729</v>
-      </c>
-      <c r="E426" t="s">
-        <v>24</v>
-      </c>
-      <c r="F426" t="s">
-        <v>41</v>
-      </c>
-      <c r="H426" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>731</v>
+        <v>288</v>
       </c>
       <c r="C427" t="s">
         <v>18</v>
       </c>
       <c r="D427" t="s">
-        <v>731</v>
+        <v>288</v>
       </c>
       <c r="E427" t="s">
         <v>20</v>
       </c>
       <c r="F427" t="s">
-        <v>693</v>
+        <v>33</v>
       </c>
       <c r="H427" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="428" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
+        <v>729</v>
+      </c>
+      <c r="C428" t="s">
+        <v>18</v>
+      </c>
+      <c r="D428" t="s">
+        <v>729</v>
+      </c>
+      <c r="E428" t="s">
+        <v>24</v>
+      </c>
+      <c r="F428" t="s">
+        <v>41</v>
+      </c>
+      <c r="H428" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B429" t="s">
+        <v>731</v>
+      </c>
+      <c r="C429" t="s">
+        <v>18</v>
+      </c>
+      <c r="D429" t="s">
+        <v>731</v>
+      </c>
+      <c r="E429" t="s">
+        <v>20</v>
+      </c>
+      <c r="F429" t="s">
+        <v>693</v>
+      </c>
+      <c r="H429" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B430" t="s">
         <v>733</v>
       </c>
-      <c r="C428" t="s">
-        <v>18</v>
-      </c>
-      <c r="D428" t="s">
+      <c r="C430" t="s">
+        <v>18</v>
+      </c>
+      <c r="D430" t="s">
         <v>733</v>
       </c>
-      <c r="E428" t="s">
-        <v>20</v>
-      </c>
-      <c r="F428" t="s">
+      <c r="E430" t="s">
+        <v>20</v>
+      </c>
+      <c r="F430" t="s">
         <v>33</v>
       </c>
-      <c r="H428" t="s">
+      <c r="H430" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A429" s="4"/>
-      <c r="B429" s="4" t="s">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A431" s="4"/>
+      <c r="B431" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C429" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D429" s="4" t="s">
+      <c r="C431" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D431" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="E429" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F429" s="5" t="s">
+      <c r="E431" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F431" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="G429" s="4"/>
-      <c r="H429" s="4" t="s">
+      <c r="G431" s="4"/>
+      <c r="H431" s="4" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A430" s="3"/>
-      <c r="B430" s="3" t="s">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A432" s="3"/>
+      <c r="B432" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="C430" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D430" s="3" t="s">
+      <c r="C432" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D432" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="E430" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F430" s="3" t="s">
+      <c r="E432" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F432" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="G430" s="3"/>
-      <c r="H430" s="3" t="s">
+      <c r="G432" s="3"/>
+      <c r="H432" s="3" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B431" t="s">
+    <row r="433" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B433" t="s">
         <v>739</v>
       </c>
-      <c r="C431" t="s">
-        <v>18</v>
-      </c>
-      <c r="D431" t="s">
+      <c r="C433" t="s">
+        <v>18</v>
+      </c>
+      <c r="D433" t="s">
         <v>739</v>
       </c>
-      <c r="E431" t="s">
-        <v>20</v>
-      </c>
-      <c r="F431" t="s">
+      <c r="E433" t="s">
+        <v>20</v>
+      </c>
+      <c r="F433" t="s">
         <v>693</v>
       </c>
-      <c r="H431" t="s">
+      <c r="H433" t="s">
         <v>742</v>
       </c>
     </row>
@@ -14145,8 +14217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>